<commit_message>
did calibration and alignment testing
</commit_message>
<xml_diff>
--- a/damn you sensors.xlsx
+++ b/damn you sensors.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ching Jia Chin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kiang\Desktop\CZ3004 codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDA76B34-7FFE-46E9-B5E6-DDEC5D5F3FD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40ABCA8-5C16-49A3-A8FE-C5A1B071BF23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="19200" windowHeight="10160" xr2:uid="{C7E69244-A8F9-48E7-9CC4-32A0FC01B222}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C7E69244-A8F9-48E7-9CC4-32A0FC01B222}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>one</t>
   </si>
@@ -41,11 +41,17 @@
   <si>
     <t>two</t>
   </si>
+  <si>
+    <t xml:space="preserve">four </t>
+  </si>
+  <si>
+    <t>five</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -81,8 +87,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{4DFBA872-9E19-4EC4-B0B4-4179A990ADEC}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -391,15 +425,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70D8498C-C742-42A4-B355-A3531E22073A}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -409,128 +443,295 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="C2">
+        <v>2.71</v>
+      </c>
+      <c r="D2">
+        <v>2.79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>5.6</v>
-      </c>
-      <c r="C2">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="B3">
+        <v>3.29</v>
+      </c>
+      <c r="C3">
+        <v>3.7</v>
+      </c>
+      <c r="D3">
+        <v>3.78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>5.6</v>
-      </c>
-      <c r="C3">
-        <v>5.6</v>
-      </c>
-      <c r="D3">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="B4">
+        <v>4.34</v>
+      </c>
+      <c r="C4">
+        <v>4.71</v>
+      </c>
+      <c r="D4">
+        <v>4.6399999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>6.2</v>
-      </c>
-      <c r="C4">
-        <v>6.6</v>
-      </c>
-      <c r="D4">
-        <v>5.9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="B5">
+        <v>5.48</v>
+      </c>
+      <c r="C5">
+        <v>5.79</v>
+      </c>
+      <c r="D5">
+        <v>5.74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>7.2</v>
-      </c>
-      <c r="C5">
-        <v>7.8</v>
-      </c>
-      <c r="D5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="B6">
+        <v>6.67</v>
+      </c>
+      <c r="C6">
+        <v>6.85</v>
+      </c>
+      <c r="D6">
+        <v>6.91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
         <v>8</v>
       </c>
-      <c r="B6">
-        <v>8.4</v>
-      </c>
-      <c r="C6">
-        <v>8.4</v>
-      </c>
-      <c r="D6">
-        <v>7.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="B7">
+        <v>7.85</v>
+      </c>
+      <c r="C7">
+        <v>7.96</v>
+      </c>
+      <c r="D7">
+        <v>7.98</v>
+      </c>
+      <c r="E7">
+        <f>+-0.3</f>
+        <v>-0.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
         <v>9</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>8.9</v>
       </c>
-      <c r="C7">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="D7">
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="C8">
+        <v>9.07</v>
+      </c>
+      <c r="D8">
+        <v>8.8699999999999992</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
         <v>10</v>
       </c>
-      <c r="B8">
-        <v>10.4</v>
-      </c>
-      <c r="C8">
-        <v>10.5</v>
-      </c>
-      <c r="D8">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="B9">
+        <v>10.029999999999999</v>
+      </c>
+      <c r="C9">
+        <v>10.07</v>
+      </c>
+      <c r="D9">
+        <v>9.92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>11.18</v>
+      </c>
+      <c r="C10">
+        <v>11.03</v>
+      </c>
+      <c r="D10">
+        <v>11.12</v>
+      </c>
+      <c r="E10">
+        <f>+-0.2</f>
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10">
+      <c r="B11">
+        <v>12.12</v>
+      </c>
+      <c r="C11">
+        <v>12.35</v>
+      </c>
+      <c r="D11">
+        <v>11.98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11">
+      <c r="B12">
+        <v>14.46</v>
+      </c>
+      <c r="C12">
+        <v>14.35</v>
+      </c>
+      <c r="D12">
+        <v>14.12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12">
+      <c r="B13">
+        <v>16.43</v>
+      </c>
+      <c r="C13">
+        <v>16.21</v>
+      </c>
+      <c r="D13">
+        <v>15.94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13">
+      <c r="B14">
+        <v>18.52</v>
+      </c>
+      <c r="C14">
+        <v>18.07</v>
+      </c>
+      <c r="D14">
+        <v>17.78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15">
         <v>20</v>
+      </c>
+      <c r="B15">
+        <v>20.56</v>
+      </c>
+      <c r="C15">
+        <v>19.98</v>
+      </c>
+      <c r="D15">
+        <v>19.54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>21.99</v>
+      </c>
+      <c r="C16">
+        <v>21.9</v>
+      </c>
+      <c r="D16">
+        <v>21.73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>24.07</v>
+      </c>
+      <c r="C17">
+        <v>23.93</v>
+      </c>
+      <c r="D17">
+        <v>24.31</v>
+      </c>
+      <c r="E17">
+        <f>+-0.8</f>
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>25.8</v>
+      </c>
+      <c r="C18">
+        <v>26.85</v>
+      </c>
+      <c r="D18">
+        <v>25.6</v>
+      </c>
+      <c r="E18">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>28</v>
+      </c>
+      <c r="B19">
+        <v>27.46</v>
+      </c>
+      <c r="C19">
+        <v>31.11</v>
+      </c>
+      <c r="D19">
+        <v>28.06</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>30</v>
+      </c>
+      <c r="B20">
+        <v>292</v>
+      </c>
+      <c r="C20">
+        <v>33.229999999999997</v>
+      </c>
+      <c r="D20">
+        <v>29.92</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commented front and backward movement for fixed distance front align
</commit_message>
<xml_diff>
--- a/damn you sensors.xlsx
+++ b/damn you sensors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kiang\Desktop\CZ3004 codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40ABCA8-5C16-49A3-A8FE-C5A1B071BF23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC29FBED-A06F-4B5E-8830-15D2F9FF5B51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C7E69244-A8F9-48E7-9CC4-32A0FC01B222}"/>
   </bookViews>
@@ -427,7 +427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70D8498C-C742-42A4-B355-A3531E22073A}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>

</xml_diff>